<commit_message>
uncomment context extension dab160d90e815c0ad7cfdc5e539965801361ac97
</commit_message>
<xml_diff>
--- a/ig/sd-modification-extension-eclairelabel-to-R5/StructureDefinition-eclaire-label-r5.xlsx
+++ b/ig/sd-modification-extension-eclairelabel-to-R5/StructureDefinition-eclaire-label-r5.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-10-31T17:23:44+00:00</t>
+    <t>2023-10-31T17:39:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -126,7 +126,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Element</t>
+    <t>element:ResearchStudy</t>
   </si>
   <si>
     <t/>

</xml_diff>